<commit_message>
updated scrum, all sprint5 tasks complete
</commit_message>
<xml_diff>
--- a/Robbie_Robot_Shop_Scrum.xlsx
+++ b/Robbie_Robot_Shop_Scrum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="627" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="627"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="190">
   <si>
     <t>Product Name:</t>
   </si>
@@ -580,18 +580,6 @@
     <t>Window with menue buttons completed 10/30/16</t>
   </si>
   <si>
-    <t>All classes are in 1 .cpp file. Need to get a working Makefile so classes can be separated into multiple files.</t>
-  </si>
-  <si>
-    <t>Not Started</t>
-  </si>
-  <si>
-    <t>PM3.1</t>
-  </si>
-  <si>
-    <t>Create a working Makefile to separate all classes in .cpp</t>
-  </si>
-  <si>
     <t>Display a dialogue box giving user propmpts</t>
   </si>
   <si>
@@ -604,10 +592,7 @@
     <t>Take user input via GUI dialogs</t>
   </si>
   <si>
-    <t>PM3.4</t>
-  </si>
-  <si>
-    <t>Save the robot parts via GUI dialogs &amp; files</t>
+    <t>Window opens with user input boxes</t>
   </si>
 </sst>
 </file>
@@ -1077,11 +1062,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2113421576"/>
-        <c:axId val="2113427176"/>
+        <c:axId val="2104176312"/>
+        <c:axId val="2104181912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2113421576"/>
+        <c:axId val="2104176312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1125,7 +1110,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2113427176"/>
+        <c:crossAx val="2104181912"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1133,7 +1118,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2113427176"/>
+        <c:axId val="2104181912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1187,7 +1172,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2113421576"/>
+        <c:crossAx val="2104176312"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1346,11 +1331,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2111759208"/>
-        <c:axId val="2111764920"/>
+        <c:axId val="2104229272"/>
+        <c:axId val="2104234984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2111759208"/>
+        <c:axId val="2104229272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1374,7 +1359,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="1"/>
         </c:title>
         <c:majorTickMark val="out"/>
@@ -1387,7 +1371,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2111764920"/>
+        <c:crossAx val="2104234984"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1395,7 +1379,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2111764920"/>
+        <c:axId val="2104234984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1449,7 +1433,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2111759208"/>
+        <c:crossAx val="2104229272"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1563,28 +1547,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>11.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1601,11 +1585,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2111082360"/>
-        <c:axId val="2111076632"/>
+        <c:axId val="2104299144"/>
+        <c:axId val="2104304856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2111082360"/>
+        <c:axId val="2104299144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1642,7 +1626,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2111076632"/>
+        <c:crossAx val="2104304856"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1650,7 +1634,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2111076632"/>
+        <c:axId val="2104304856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1704,7 +1688,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2111082360"/>
+        <c:crossAx val="2104299144"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2168,8 +2152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2687,6 +2671,9 @@
       <c r="B34">
         <v>1</v>
       </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
       <c r="E34" s="1">
         <v>1</v>
       </c>
@@ -2730,6 +2717,9 @@
       <c r="B36">
         <v>3</v>
       </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
       <c r="E36" s="1">
         <v>1</v>
       </c>
@@ -3439,7 +3429,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -3771,10 +3760,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3858,7 +3847,7 @@
         <v>135</v>
       </c>
       <c r="B6" s="32">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -3872,8 +3861,7 @@
         <v>136</v>
       </c>
       <c r="B7" s="32">
-        <f t="shared" ref="B7:B12" si="0">B6</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -3887,8 +3875,7 @@
         <v>137</v>
       </c>
       <c r="B8" s="32">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -3902,8 +3889,7 @@
         <v>138</v>
       </c>
       <c r="B9" s="32">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -3917,7 +3903,7 @@
         <v>139</v>
       </c>
       <c r="B10" s="32">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -3931,8 +3917,7 @@
         <v>140</v>
       </c>
       <c r="B11" s="32">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -3946,8 +3931,7 @@
         <v>141</v>
       </c>
       <c r="B12" s="32">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -3961,8 +3945,7 @@
         <v>142</v>
       </c>
       <c r="B13" s="32">
-        <f>B12</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -4169,12 +4152,12 @@
         <v>36</v>
       </c>
       <c r="G24" s="43" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="34" customFormat="1">
+      <c r="A25" s="43" t="s">
         <v>186</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="34" customFormat="1" ht="36">
-      <c r="A25" s="43" t="s">
-        <v>187</v>
       </c>
       <c r="B25" s="43" t="s">
         <v>154</v>
@@ -4185,20 +4168,22 @@
       <c r="D25" s="43" t="s">
         <v>182</v>
       </c>
-      <c r="E25" s="43"/>
+      <c r="E25" s="43" t="s">
+        <v>152</v>
+      </c>
       <c r="F25" s="12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G25" s="43" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="H25" s="34" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="34" customFormat="1">
       <c r="A26" s="43" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B26" s="43" t="s">
         <v>154</v>
@@ -4209,56 +4194,21 @@
       <c r="D26" s="43" t="s">
         <v>182</v>
       </c>
-      <c r="E26" s="43"/>
-      <c r="F26" s="12" t="s">
+      <c r="E26" s="43" t="s">
+        <v>152</v>
+      </c>
+      <c r="F26" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="G26" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="H26" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="G26" s="43" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="34" customFormat="1">
-      <c r="A27" s="43" t="s">
-        <v>191</v>
-      </c>
-      <c r="B27" s="43" t="s">
-        <v>154</v>
-      </c>
-      <c r="C27" s="43" t="s">
-        <v>183</v>
-      </c>
-      <c r="D27" s="43" t="s">
-        <v>182</v>
-      </c>
-      <c r="E27" s="43"/>
-      <c r="F27" s="34" t="s">
-        <v>192</v>
-      </c>
-      <c r="G27" s="43" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="34" customFormat="1">
-      <c r="A28" s="43" t="s">
-        <v>193</v>
-      </c>
-      <c r="B28" s="43" t="s">
-        <v>154</v>
-      </c>
-      <c r="C28" s="43" t="s">
-        <v>183</v>
-      </c>
-      <c r="D28" s="43" t="s">
-        <v>182</v>
-      </c>
-      <c r="E28" s="43"/>
-      <c r="F28" s="34" t="s">
-        <v>194</v>
-      </c>
-      <c r="G28" s="43" t="s">
-        <v>186</v>
-      </c>
-    </row>
+    </row>
+    <row r="27" spans="1:8" s="34" customFormat="1"/>
+    <row r="28" spans="1:8" s="34" customFormat="1"/>
     <row r="29" spans="1:8" s="34" customFormat="1"/>
     <row r="30" spans="1:8" s="34" customFormat="1"/>
     <row r="31" spans="1:8" s="34" customFormat="1"/>
@@ -4275,11 +4225,8 @@
     <row r="42" s="34" customFormat="1"/>
     <row r="43" s="34" customFormat="1"/>
     <row r="44" s="34" customFormat="1"/>
-    <row r="45" s="34" customFormat="1"/>
-    <row r="46" s="34" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>